<commit_message>
product quantity bug fix
</commit_message>
<xml_diff>
--- a/public/SRexcel/sales-report-${formattedStartDate}-${formattedEndDate}.xlsx
+++ b/public/SRexcel/sales-report-${formattedStartDate}-${formattedEndDate}.xlsx
@@ -11,14 +11,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Order ID</t>
   </si>
   <si>
-    <t>Product Name</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -28,34 +25,55 @@
     <t>Payment Method</t>
   </si>
   <si>
-    <t>VLCZU1DC</t>
-  </si>
-  <si>
-    <t>APPLE AirPods Pro</t>
-  </si>
-  <si>
-    <t>22/1/2024</t>
+    <t>DPRJV1CL</t>
+  </si>
+  <si>
+    <t>23/1/2024</t>
+  </si>
+  <si>
+    <t>87945.00</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>WVAJ27DU</t>
+  </si>
+  <si>
+    <t>24/1/2024</t>
+  </si>
+  <si>
+    <t>108945.00</t>
+  </si>
+  <si>
+    <t>4A690OVT</t>
+  </si>
+  <si>
+    <t>BA8WTN90</t>
+  </si>
+  <si>
+    <t>24500.00</t>
+  </si>
+  <si>
+    <t>05ZJMUH8</t>
   </si>
   <si>
     <t>21000.00</t>
   </si>
   <si>
-    <t>COD</t>
-  </si>
-  <si>
-    <t>Y5Y63RUL</t>
-  </si>
-  <si>
-    <t>Apple Tv</t>
-  </si>
-  <si>
-    <t>24500.00</t>
+    <t>136J6JJT</t>
+  </si>
+  <si>
+    <t>25/1/2024</t>
+  </si>
+  <si>
+    <t>320442.00</t>
   </si>
   <si>
     <t>Total Sales Amount</t>
   </si>
   <si>
-    <t>45500.00</t>
+    <t>650777.00</t>
   </si>
 </sst>
 </file>
@@ -432,13 +450,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="5" width="25" customWidth="1"/>
+    <col min="1" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,50 +469,97 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>